<commit_message>
april frame done.refactor logic in accessory_frame. there are some little bugs
</commit_message>
<xml_diff>
--- a/months/apr23/apr23.xlsx
+++ b/months/apr23/apr23.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="vedomost" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="169">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -257,6 +257,24 @@
   </si>
   <si>
     <t xml:space="preserve">23:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1,L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E4,L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23:12</t>
   </si>
   <si>
     <t xml:space="preserve">штрафы</t>
@@ -656,7 +674,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -710,6 +728,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -947,15 +969,15 @@
   </sheetPr>
   <dimension ref="A1:AH32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="K30" activeCellId="0" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="4.43"/>
@@ -984,7 +1006,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="4" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="5" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="5.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="7.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="33" min="33" style="4" width="8.57"/>
   </cols>
@@ -3090,36 +3112,83 @@
         <f aca="false">IFERROR(WEEKDAY(A28,2),"")</f>
         <v>4</v>
       </c>
-      <c r="C28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="F28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
+      <c r="H28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="8"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="10"/>
+      <c r="Q28" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="S28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T28" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="U28" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="V28" s="10"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="7"/>
-      <c r="Y28" s="7"/>
-      <c r="Z28" s="7"/>
-      <c r="AA28" s="8"/>
-      <c r="AB28" s="10"/>
+      <c r="W28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="X28" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA28" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB28" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="AC28" s="3"/>
-      <c r="AD28" s="7"/>
+      <c r="AD28" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE28" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF28" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="n">
@@ -3129,30 +3198,65 @@
         <f aca="false">IFERROR(WEEKDAY(A29,2),"")</f>
         <v>5</v>
       </c>
-      <c r="C29" s="7"/>
+      <c r="C29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="H29" s="9"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
+      <c r="I29" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
+      <c r="O29" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="P29" s="8"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="10"/>
+      <c r="Q29" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="S29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T29" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="U29" s="10"/>
-      <c r="V29" s="10"/>
+      <c r="V29" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="W29" s="7"/>
-      <c r="X29" s="7"/>
+      <c r="X29" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="Y29" s="7"/>
-      <c r="Z29" s="7"/>
-      <c r="AA29" s="8"/>
+      <c r="Z29" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA29" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="AB29" s="10"/>
       <c r="AC29" s="3"/>
-      <c r="AD29" s="7"/>
+      <c r="AD29" s="7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="n">
@@ -3162,30 +3266,68 @@
         <f aca="false">IFERROR(WEEKDAY(A30,2),"")</f>
         <v>6</v>
       </c>
-      <c r="C30" s="7"/>
+      <c r="C30" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="H30" s="9"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
+      <c r="I30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="M30" s="7"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
+      <c r="O30" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="P30" s="8"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="10"/>
+      <c r="Q30" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="R30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="S30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T30" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="U30" s="10"/>
       <c r="V30" s="10"/>
       <c r="W30" s="7"/>
-      <c r="X30" s="7"/>
-      <c r="Y30" s="7"/>
-      <c r="Z30" s="7"/>
-      <c r="AA30" s="8"/>
-      <c r="AB30" s="10"/>
+      <c r="X30" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB30" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="AC30" s="3"/>
-      <c r="AD30" s="7"/>
+      <c r="AD30" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF30" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="n">
@@ -3267,7 +3409,7 @@
       <formula>LEFT(A26,LEN("!"))="!"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="40">
+  <dataValidations count="27">
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Время сна Арины" promptTitle="синтаксис: число,число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I32" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -3304,7 +3446,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Выполнение задания&#10;E - ЕГР&#10;L - ЛЕРА" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N32" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Выполнение задания&#10;E - ЕГР&#10;L - ЛЕРА" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N2:N7 N9:N32" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3316,19 +3458,19 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Чистка зубов Леры. &#10;T - да&#10;9 - чистка до 9 утра" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AA2:AB25 AA28:AB31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Чистка зубов Леры. &#10;T - да&#10;9 - чистка до 9 утра" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AA2:AB31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Кодируем дефицит сна&#10;C - не выспался из-за детей&#10;D - не выспался на дежурстве&#10;I - бессонница&#10;F - не выспался по сем. делам&#10;P - не выспался, развлекался&#10;&#10;&quot;+&quot; если был сон, &quot;-&quot; ели не было&#10;например: +С" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА+" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC2:AC25 AC28:AC31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Кодируем дефицит сна&#10;C - не выспался из-за детей&#10;D - не выспался на дежурстве&#10;I - бессонница&#10;F - не выспался по сем. делам&#10;P - не выспался, развлекался&#10;&#10;&quot;+&quot; если был сон, &quot;-&quot; ели не было&#10;например: +С" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА+" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC2:AC31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Время сна Леры" promptTitle="синтаксис: число:число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD2:AD25 AD28:AD31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Время сна Леры" promptTitle="синтаксис: число:число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD2:AD31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Без перекусов, Лера!&#10;T - да" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AE2:AE25 AE28:AE31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Без перекусов, Лера!&#10;T - да" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AE2:AE31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3344,87 +3486,35 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="число мл жидкости, выпоенной аришке" promptTitle="синтаксис: число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H7 H9:H25 H28:H31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="число мл жидкости, выпоенной аришке" promptTitle="синтаксис: число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H2:H7 H9:H31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Время сна Арины" promptTitle="синтаксис: число:число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I2:I7 I9:I25 I28:I31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Время сна Арины" promptTitle="синтаксис: число:число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I2:I7 I9:I31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Время сна Златы" promptTitle="синтаксис: число:число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K7 K9:K25 K28:K31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Время сна Златы" promptTitle="синтаксис: число:число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K7 K9:K31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Сколько снов у Златы" promptTitle="синтаксис: число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L2:L7 L9:L25 L28:L31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Сколько снов у Златы" promptTitle="синтаксис: число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L2:L7 L9:L31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Чистка зубов Златы. &#10;T - да&#10;" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M2:M7 M9:M25 M28:M31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Чистка зубов Златы. &#10;T - да&#10;" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M2:M7 M9:M31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Выполнение задания&#10;E - ЕГР&#10;L - ЛЕРА" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N2:N7 N9:N25 N28:N31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Без телевизера&#10;T - да" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O2:O7 O9:O31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Без телевизера&#10;T - да" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O2:O7 O9:O25 O28:O31" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Убранная кухня&#10;T - да" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R2:R7 R9:R25 R28:R31" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Убранная кухня&#10;T - да" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R2:R7 R9:R31" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Выполнение ранее запланированных заданий. Кто сколько сделал:&#10;L1,E5 например" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВАчисло" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T2:T19" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Убранная кухня&#10;T - да" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R26:R27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Без телевизера&#10;T - да" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="O26:O27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Выполнение задания&#10;E - ЕГР&#10;L - ЛЕРА" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="N26:N27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Чистка зубов Златы. &#10;T - да&#10;" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M26:M27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Сколько снов у Златы" promptTitle="синтаксис: число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L26:L27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Время сна Златы" promptTitle="синтаксис: число:число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K26:K27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Время сна Арины" promptTitle="синтаксис: число:число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I26:I27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="число мл жидкости, выпоенной аришке" promptTitle="синтаксис: число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H26:H27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Без перекусов, Лера!&#10;T - да" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AE26:AE27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Время сна Леры" promptTitle="синтаксис: число:число" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD26:AD27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Кодируем дефицит сна&#10;C - не выспался из-за детей&#10;D - не выспался на дежурстве&#10;I - бессонница&#10;F - не выспался по сем. делам&#10;P - не выспался, развлекался&#10;&#10;&quot;+&quot; если был сон, &quot;-&quot; ели не было&#10;например: +С" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА+" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC26:AC27" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Чистка зубов Леры. &#10;T - да&#10;9 - чистка до 9 утра" promptTitle="синтаксис: ЗАГЛАВНАЯ БУКВА" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AA26:AB27" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3450,7 +3540,7 @@
       <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="12.14"/>
@@ -3459,91 +3549,91 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="A1" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
-        <v>81</v>
+      <c r="A2" s="17" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
-        <v>82</v>
+      <c r="A3" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>83</v>
+      <c r="A4" s="18" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>84</v>
+      <c r="A5" s="18" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>85</v>
+      <c r="A6" s="18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
-        <v>86</v>
+      <c r="A7" s="18" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>87</v>
+      <c r="A8" s="18" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
-        <v>88</v>
+      <c r="A9" s="19" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
-        <v>89</v>
+      <c r="A10" s="19" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>90</v>
+      <c r="A11" s="18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3586,437 +3676,437 @@
   </sheetPr>
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topRight" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="41.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="19" width="37.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="19" width="16.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="19" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="19" width="5.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="19" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="20" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="19" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="19" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="20" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="19" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="21" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="19" width="47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="19" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="19" width="33.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="19" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="20" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="19" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="19" width="45.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="19" width="33.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="19" width="5.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="26" style="19" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="41.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="21" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="37.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="16.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="5.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="21" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="20" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="20" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="21" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="20" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="22" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="20" width="47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="20" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="20" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="20" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="21" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="20" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="20" width="45.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="20" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="20" width="6.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="26" style="20" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
-        <v>96</v>
+      <c r="A1" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="W1" s="10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>122</v>
+      <c r="A2" s="24" t="s">
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>124</v>
+        <v>129</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>130</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="19" t="n">
+        <v>131</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="20" t="n">
         <v>50</v>
       </c>
-      <c r="H2" s="19" t="n">
+      <c r="H2" s="20" t="n">
         <v>50</v>
       </c>
-      <c r="I2" s="24" t="n">
+      <c r="I2" s="25" t="n">
         <v>150</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="L2" s="24" t="n">
+        <v>133</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="25" t="n">
         <v>50</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q2" s="24" t="n">
+        <v>134</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q2" s="25" t="n">
         <v>50</v>
       </c>
-      <c r="R2" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="S2" s="19" t="n">
+      <c r="R2" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="S2" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="T2" s="24" t="s">
-        <v>129</v>
+      <c r="T2" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="V2" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="W2" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="X2" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y2" s="19" t="n">
+        <v>139</v>
+      </c>
+      <c r="V2" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="X2" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y2" s="20" t="n">
         <v>50</v>
       </c>
-      <c r="Z2" s="19" t="s">
-        <v>130</v>
+      <c r="Z2" s="20" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
-        <v>136</v>
+      <c r="A3" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="B3" s="12" t="n">
         <v>-25</v>
       </c>
-      <c r="C3" s="24" t="n">
+      <c r="C3" s="25" t="n">
         <v>-50</v>
       </c>
       <c r="D3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="24" t="n">
+      <c r="E3" s="25" t="n">
         <v>50</v>
       </c>
-      <c r="F3" s="24" t="n">
+      <c r="F3" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="19" t="n">
+      <c r="G3" s="20" t="n">
         <v>-50</v>
       </c>
-      <c r="H3" s="19" t="n">
+      <c r="H3" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="I3" s="24" t="n">
+      <c r="I3" s="25" t="n">
         <v>-25</v>
       </c>
       <c r="J3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24" t="n">
+      <c r="K3" s="25"/>
+      <c r="L3" s="25" t="n">
         <v>-50</v>
       </c>
       <c r="M3" s="12" t="n">
         <v>-50</v>
       </c>
-      <c r="N3" s="24" t="n">
+      <c r="N3" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="O3" s="24" t="n">
+      <c r="O3" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="P3" s="24" t="n">
+      <c r="P3" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" s="24" t="n">
+      <c r="Q3" s="25" t="n">
         <v>-50</v>
       </c>
-      <c r="R3" s="24" t="n">
+      <c r="R3" s="25" t="n">
         <v>-50</v>
       </c>
-      <c r="S3" s="19" t="n">
+      <c r="S3" s="20" t="n">
         <v>-50</v>
       </c>
-      <c r="T3" s="24" t="n">
+      <c r="T3" s="25" t="n">
         <v>0</v>
       </c>
       <c r="U3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="V3" s="24" t="n">
+      <c r="V3" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="W3" s="24" t="n">
+      <c r="W3" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="X3" s="24" t="n">
+      <c r="X3" s="25" t="n">
         <v>-50</v>
       </c>
-      <c r="Y3" s="19" t="n">
+      <c r="Y3" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="Z3" s="19" t="n">
+      <c r="Z3" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
-        <v>137</v>
+      <c r="A4" s="26" t="s">
+        <v>143</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>138</v>
+        <v>129</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>144</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="19" t="n">
+        <v>131</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="19" t="n">
+      <c r="H4" s="20" t="n">
         <v>50</v>
       </c>
-      <c r="I4" s="24" t="n">
+      <c r="I4" s="25" t="n">
         <v>50</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="L4" s="24" t="n">
+        <v>136</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="L4" s="25" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="O4" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="P4" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q4" s="24" t="n">
+        <v>147</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="P4" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q4" s="25" t="n">
         <v>100</v>
       </c>
-      <c r="R4" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="S4" s="19" t="n">
+      <c r="R4" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="S4" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="T4" s="24" t="s">
-        <v>130</v>
+      <c r="T4" s="25" t="s">
+        <v>136</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="V4" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="W4" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="X4" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y4" s="19" t="n">
+        <v>147</v>
+      </c>
+      <c r="V4" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="W4" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="X4" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y4" s="20" t="n">
         <v>50</v>
       </c>
-      <c r="Z4" s="19" t="s">
-        <v>129</v>
+      <c r="Z4" s="20" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
-        <v>144</v>
+      <c r="A5" s="26" t="s">
+        <v>150</v>
       </c>
       <c r="B5" s="12" t="n">
         <v>-25</v>
       </c>
-      <c r="C5" s="24" t="n">
+      <c r="C5" s="25" t="n">
         <v>-50</v>
       </c>
       <c r="D5" s="12" t="n">
         <v>-50</v>
       </c>
-      <c r="E5" s="24" t="n">
+      <c r="E5" s="25" t="n">
         <v>-50</v>
       </c>
-      <c r="F5" s="24" t="n">
+      <c r="F5" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="19" t="n">
+      <c r="G5" s="20" t="n">
         <v>-50</v>
       </c>
-      <c r="H5" s="19" t="n">
+      <c r="H5" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="24" t="n">
+      <c r="I5" s="25" t="n">
         <v>-50</v>
       </c>
       <c r="J5" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24" t="n">
+      <c r="K5" s="25"/>
+      <c r="L5" s="25" t="n">
         <v>-50</v>
       </c>
       <c r="M5" s="12" t="n">
         <v>-50</v>
       </c>
-      <c r="N5" s="24" t="n">
+      <c r="N5" s="25" t="n">
         <v>-50</v>
       </c>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24" t="n">
+      <c r="O5" s="25"/>
+      <c r="P5" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" s="24" t="n">
+      <c r="Q5" s="25" t="n">
+        <v>-25</v>
+      </c>
+      <c r="R5" s="25" t="n">
         <v>-50</v>
       </c>
-      <c r="R5" s="24" t="n">
+      <c r="S5" s="20" t="n">
         <v>-50</v>
       </c>
-      <c r="S5" s="19" t="n">
-        <v>-50</v>
-      </c>
-      <c r="T5" s="24" t="n">
+      <c r="T5" s="25" t="n">
         <v>0</v>
       </c>
       <c r="U5" s="12" t="n">
         <v>-50</v>
       </c>
-      <c r="V5" s="24" t="n">
+      <c r="V5" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="W5" s="24" t="n">
+      <c r="W5" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="X5" s="24" t="n">
+      <c r="X5" s="25" t="n">
         <v>-50</v>
       </c>
-      <c r="Y5" s="19" t="n">
+      <c r="Y5" s="20" t="n">
         <v>-50</v>
       </c>
-      <c r="Z5" s="19" t="n">
+      <c r="Z5" s="20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4" t="n">
@@ -4034,10 +4124,10 @@
       <c r="F6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="19" t="n">
+      <c r="G6" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="20" t="n">
         <v>1</v>
       </c>
       <c r="I6" s="5" t="n">
@@ -4053,28 +4143,28 @@
         <v>1</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="O6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="S6" s="19" t="s">
-        <v>145</v>
+        <v>151</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>151</v>
       </c>
       <c r="T6" s="5" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="U6" s="4" t="n">
         <v>1</v>
@@ -4088,16 +4178,16 @@
       <c r="X6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="Y6" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="19" t="n">
+      <c r="Y6" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="20" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
-        <v>146</v>
+      <c r="A7" s="28" t="s">
+        <v>152</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>0.75</v>
@@ -4178,8 +4268,8 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28" t="s">
-        <v>147</v>
+      <c r="A8" s="29" t="s">
+        <v>153</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>1.25</v>
@@ -4196,10 +4286,10 @@
       <c r="F8" s="5" t="n">
         <v>1.25</v>
       </c>
-      <c r="G8" s="19" t="n">
+      <c r="G8" s="20" t="n">
         <v>1.25</v>
       </c>
-      <c r="H8" s="19" t="n">
+      <c r="H8" s="20" t="n">
         <v>1.25</v>
       </c>
       <c r="I8" s="5" t="n">
@@ -4232,7 +4322,7 @@
       <c r="R8" s="5" t="n">
         <v>1.25</v>
       </c>
-      <c r="S8" s="19" t="n">
+      <c r="S8" s="20" t="n">
         <v>1.25</v>
       </c>
       <c r="T8" s="5" t="n">
@@ -4250,16 +4340,16 @@
       <c r="X8" s="5" t="n">
         <v>1.25</v>
       </c>
-      <c r="Y8" s="19" t="n">
+      <c r="Y8" s="20" t="n">
         <v>1.25</v>
       </c>
-      <c r="Z8" s="19" t="n">
+      <c r="Z8" s="20" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="28" t="s">
-        <v>148</v>
+      <c r="A9" s="29" t="s">
+        <v>154</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>1.5</v>
@@ -4276,10 +4366,10 @@
       <c r="F9" s="5" t="n">
         <v>1.5</v>
       </c>
-      <c r="G9" s="19" t="n">
+      <c r="G9" s="20" t="n">
         <v>1.5</v>
       </c>
-      <c r="H9" s="19" t="n">
+      <c r="H9" s="20" t="n">
         <v>1.5</v>
       </c>
       <c r="I9" s="5" t="n">
@@ -4312,7 +4402,7 @@
       <c r="R9" s="5" t="n">
         <v>1.5</v>
       </c>
-      <c r="S9" s="19" t="n">
+      <c r="S9" s="20" t="n">
         <v>1.5</v>
       </c>
       <c r="T9" s="5" t="n">
@@ -4330,22 +4420,22 @@
       <c r="X9" s="5" t="n">
         <v>1.5</v>
       </c>
-      <c r="Y9" s="19" t="n">
+      <c r="Y9" s="20" t="n">
         <v>1.5</v>
       </c>
-      <c r="Z9" s="19" t="n">
+      <c r="Z9" s="20" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="30" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>0.5</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>0.5</v>
@@ -4356,10 +4446,10 @@
       <c r="F10" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="19" t="n">
+      <c r="G10" s="20" t="n">
         <v>0.5</v>
       </c>
-      <c r="H10" s="19" t="n">
+      <c r="H10" s="20" t="n">
         <v>0.5</v>
       </c>
       <c r="I10" s="5" t="n">
@@ -4392,7 +4482,7 @@
       <c r="R10" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="S10" s="19" t="n">
+      <c r="S10" s="20" t="n">
         <v>0.5</v>
       </c>
       <c r="T10" s="5" t="n">
@@ -4410,16 +4500,16 @@
       <c r="X10" s="5" t="n">
         <v>0.5</v>
       </c>
-      <c r="Y10" s="19" t="n">
+      <c r="Y10" s="20" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z10" s="19" t="n">
+      <c r="Z10" s="20" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29" t="s">
-        <v>149</v>
+      <c r="A11" s="30" t="s">
+        <v>155</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>0.75</v>
@@ -4436,10 +4526,10 @@
       <c r="F11" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="19" t="n">
+      <c r="G11" s="20" t="n">
         <v>0.75</v>
       </c>
-      <c r="H11" s="19" t="n">
+      <c r="H11" s="20" t="n">
         <v>0.75</v>
       </c>
       <c r="I11" s="5" t="n">
@@ -4472,7 +4562,7 @@
       <c r="R11" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="S11" s="19" t="n">
+      <c r="S11" s="20" t="n">
         <v>0.75</v>
       </c>
       <c r="T11" s="5" t="n">
@@ -4490,202 +4580,202 @@
       <c r="X11" s="5" t="n">
         <v>0.75</v>
       </c>
-      <c r="Y11" s="19" t="n">
+      <c r="Y11" s="20" t="n">
         <v>0.75</v>
       </c>
-      <c r="Z11" s="19" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
+      <c r="Z11" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="20" t="n">
+      <c r="B12" s="21" t="n">
         <v>1.25</v>
       </c>
-      <c r="C12" s="20" t="n">
+      <c r="C12" s="21" t="n">
         <v>1.25</v>
       </c>
-      <c r="D12" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="20" t="n">
+      <c r="D12" s="21" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E12" s="21" t="n">
         <v>1.25</v>
       </c>
-      <c r="F12" s="20" t="n">
+      <c r="F12" s="21" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G12" s="21" t="n">
         <v>1.25</v>
       </c>
-      <c r="G12" s="20" t="n">
+      <c r="H12" s="21" t="n">
         <v>1.25</v>
       </c>
-      <c r="H12" s="20" t="n">
+      <c r="I12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="21" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K12" s="21" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="L12" s="21" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M12" s="21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O12" s="21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P12" s="21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q12" s="21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R12" s="21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S12" s="21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T12" s="21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U12" s="21" t="n">
         <v>1.25</v>
       </c>
-      <c r="I12" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="20" t="n">
+      <c r="V12" s="21" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="W12" s="21" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="X12" s="21" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="Y12" s="21" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="Z12" s="21" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="21" t="n">
         <v>0.75</v>
       </c>
-      <c r="K12" s="20" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="L12" s="20" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="M12" s="20" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N12" s="20" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="O12" s="20" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="P12" s="20" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Q12" s="20" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="R12" s="20" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="S12" s="20" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="T12" s="20" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="U12" s="20" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="V12" s="20" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="W12" s="20" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="X12" s="20" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="Y12" s="20" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="Z12" s="20" t="n">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="B13" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="20" t="n">
+      <c r="E13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="K13" s="19" t="n">
+      <c r="K13" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="L13" s="19" t="n">
+      <c r="L13" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="M13" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="P13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="R13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="S13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="T13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="U13" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="V13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="W13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="X13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="19" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="19" t="n">
+      <c r="M13" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="S13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="T13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="U13" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="V13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="W13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="X13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="20" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H16" s="21"/>
+      <c r="H16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H17" s="21"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="21"/>
+      <c r="H18" s="22"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="21"/>
+      <c r="H19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="21"/>
+      <c r="H20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H21" s="21"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="21"/>
+      <c r="H22" s="22"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H23" s="21"/>
+      <c r="H23" s="22"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="21"/>
+      <c r="H24" s="22"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H25" s="21"/>
+      <c r="H25" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="AA6:AMJ13 A6:U11 W6:Z11 W13:Z13 A13:U13 A12:Z12">
@@ -4719,7 +4809,7 @@
       <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="5.43"/>
@@ -4739,7 +4829,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="7.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="3" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="3" width="7.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="3" width="6.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="3" width="9.14"/>
@@ -4747,7 +4837,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -4875,16 +4965,16 @@
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="G2" s="3" t="n">
         <v>1</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>13</v>
@@ -4893,7 +4983,7 @@
         <v>13</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>14</v>
@@ -4923,7 +5013,7 @@
         <v>14</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>14</v>
@@ -4935,7 +5025,7 @@
         <v>1</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="Z2" s="0" t="n">
         <v>1</v>
@@ -4952,7 +5042,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>2</v>
@@ -4961,16 +5051,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="G3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>9</v>
@@ -4979,13 +5069,13 @@
         <v>9</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="W3" s="3" t="n">
         <v>2</v>
@@ -4994,7 +5084,7 @@
         <v>2</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="Z3" s="0" t="n">
         <v>2</v>
@@ -5011,28 +5101,28 @@
         <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="W4" s="3" t="n">
         <v>3</v>
@@ -5041,7 +5131,7 @@
         <v>3</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="Z4" s="0" t="n">
         <v>3</v>
@@ -5055,31 +5145,31 @@
         <v>4</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="W5" s="3" t="n">
         <v>4</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="AB5" s="3" t="n">
         <v>4</v>
@@ -5090,28 +5180,28 @@
         <v>5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5120,61 +5210,61 @@
       </c>
       <c r="F7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="F8" s="32"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="31"/>
-      <c r="H10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="H10" s="32"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="31"/>
-      <c r="H11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="H11" s="32"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="31"/>
-      <c r="H12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="H12" s="32"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="31"/>
-      <c r="H13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="F16" s="32"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="H18" s="32"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>